<commit_message>
Add button for downloading excel template
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="108">
   <si>
     <t>Id of contact section</t>
   </si>
@@ -303,15 +303,6 @@
   </si>
   <si>
     <t>I am an engineer with 10+ years of research and teaching experience, with a solid background in statistics, spatial data analysis, and modelling. My main research area is environmental science, with a particular interest in natural hazards and climate change.</t>
-  </si>
-  <si>
-    <t>industy_experience_aside</t>
-  </si>
-  <si>
-    <t>teaching_experience_aside</t>
-  </si>
-  <si>
-    <t>data_science_writing_aside</t>
   </si>
   <si>
     <t>Year of entry.</t>
@@ -780,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,21 +806,6 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -839,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1108,7 +1084,7 @@
         <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
         <v>62</v>
@@ -1244,7 +1220,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1297,10 +1273,10 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
         <v>27</v>
@@ -1308,19 +1284,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -1328,7 +1304,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>70</v>
@@ -1348,10 +1324,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>73</v>
@@ -1368,7 +1344,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -1388,7 +1364,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
@@ -1434,7 +1410,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>84</v>
@@ -1442,18 +1418,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add imagen and update CV
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
@@ -773,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1223,7 +1223,7 @@
         <v>106</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Get introduction text from excel
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EB80039-0416-44AA-9A87-DC301EBA382C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
@@ -302,58 +303,58 @@
     <t>intro</t>
   </si>
   <si>
+    <t>Year of entry.</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>Link to publication</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>The first version of the Pan-European Indoor Radon Map</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>mother tongue</t>
+  </si>
+  <si>
+    <t>fluent. It has been my everyday work language since 2016</t>
+  </si>
+  <si>
+    <t>R-Shiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regional Workshop on Development of Radon Maps and the Definition of Radon Prone Areas </t>
+  </si>
+  <si>
     <t>I am an engineer with 10+ years of research and teaching experience, with a solid background in statistics, spatial data analysis, and modelling. My main research area is environmental science, with a particular interest in natural hazards and climate change.</t>
-  </si>
-  <si>
-    <t>Year of entry.</t>
-  </si>
-  <si>
-    <t>doi</t>
-  </si>
-  <si>
-    <t>Link to publication</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>journal</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>article</t>
-  </si>
-  <si>
-    <t>The first version of the Pan-European Indoor Radon Map</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>mother tongue</t>
-  </si>
-  <si>
-    <t>fluent. It has been my everyday work language since 2016</t>
-  </si>
-  <si>
-    <t>R-Shiny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional Workshop on Development of Radon Maps and the Definition of Radon Prone Areas </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -667,7 +668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -770,11 +771,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,7 +804,7 @@
         <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -812,7 +813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1084,7 +1085,7 @@
         <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>62</v>
@@ -1185,10 +1186,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1220,7 +1221,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1248,7 +1249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1273,10 +1274,10 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
         <v>27</v>
@@ -1284,19 +1285,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -1304,7 +1305,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
         <v>70</v>
@@ -1324,10 +1325,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>73</v>
@@ -1344,7 +1345,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -1364,7 +1365,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
@@ -1388,7 +1389,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1410,7 +1411,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>84</v>
@@ -1418,18 +1419,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add second page sidebar with packages
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74B41A26-918D-477C-8ECC-3290A812729D}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE367ED6-B1CD-4406-9FBA-D2EF536FA2D8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="software" sheetId="3" r:id="rId4"/>
     <sheet name="publications" sheetId="5" r:id="rId5"/>
     <sheet name="languages" sheetId="6" r:id="rId6"/>
+    <sheet name="packages" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
   <si>
     <t>Id of contact section</t>
   </si>
@@ -358,16 +359,75 @@
   </si>
   <si>
     <t>[ORCID](https://orcid.org/0000-0003-0624-2345)</t>
+  </si>
+  <si>
+    <t>Name of package</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Description of the package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description   </t>
+  </si>
+  <si>
+    <t>dangeo</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/dangeo.git</t>
+  </si>
+  <si>
+    <t>ggpyramid</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/ggpyramid.git</t>
+  </si>
+  <si>
+    <t>ggrugby</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/ggrugby.git</t>
+  </si>
+  <si>
+    <t>safecastR</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/safecastR.git</t>
+  </si>
+  <si>
+    <t>R package for accessing the Danish Map Supply Download via the kortforsyningen FTP</t>
+  </si>
+  <si>
+    <t>R function for plotting population pyramids in {ggplot2}</t>
+  </si>
+  <si>
+    <t>R functions for plotting rugby events in {ggplot2}</t>
+  </si>
+  <si>
+    <t>R package for loading data from Safecast API</t>
+  </si>
+  <si>
+    <t>package</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,17 +450,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -681,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1423,12 +1486,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A6" sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1467,4 +1531,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D44DE69-A15C-42A4-AF08-B8E341772670}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{AFFF0D05-2980-4E8D-8084-DB5D3AF76D49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Render long CV with cv_long.rmd
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="166" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B973755C-953F-41BA-8FD6-0CE8FD449929}"/>
+  <xr:revisionPtr revIDLastSave="669" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C0B95F8-DE01-49C4-8E44-45819BE16291}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
     <sheet name="text_blocks" sheetId="4" r:id="rId2"/>
     <sheet name="entries_data" sheetId="2" r:id="rId3"/>
     <sheet name="software" sheetId="3" r:id="rId4"/>
-    <sheet name="publications" sheetId="5" r:id="rId5"/>
-    <sheet name="languages" sheetId="6" r:id="rId6"/>
+    <sheet name="languages" sheetId="6" r:id="rId5"/>
+    <sheet name="publications" sheetId="5" r:id="rId6"/>
     <sheet name="packages" sheetId="7" r:id="rId7"/>
     <sheet name="apps" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="284">
   <si>
     <t>Id of contact section</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Location the entry occured</t>
   </si>
   <si>
-    <t>Primary institution affiliation for entry</t>
-  </si>
-  <si>
     <t>Start date of entry (year)</t>
   </si>
   <si>
@@ -215,235 +212,674 @@
     <t>teaching</t>
   </si>
   <si>
+    <t>Teaching assistant, 10 day geological residential fieldschool in SE Spain, Trinity College Dublin, School of Natural Sciences, Geology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application of airborne radiometric surveys for large scale geogenic radon potential classification </t>
+  </si>
+  <si>
+    <t>Journal of the European Radon Association</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.35815/radon.v1.4358</t>
+  </si>
+  <si>
+    <t>Natural Hazards and Earth System Sciences</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.5194/nhess-19-2451-2019</t>
+  </si>
+  <si>
+    <t>Estimation of residential radon exposure and definition of Radon Priority Areas based on expected lung cancer incidence</t>
+  </si>
+  <si>
+    <t>Environment International</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.envint.2018.02.025</t>
+  </si>
+  <si>
+    <t>Logistic regression model for detecting radon prone areas in Ireland</t>
+  </si>
+  <si>
+    <t>Science of the Total Environment</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.scitotenv.2017.05.071</t>
+  </si>
+  <si>
+    <t>Name of language</t>
+  </si>
+  <si>
+    <t>Relative numeric level of skill</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>ArcGIS</t>
+  </si>
+  <si>
+    <t>QGIS</t>
+  </si>
+  <si>
+    <t>Id used for finding text block</t>
+  </si>
+  <si>
+    <t>Contents of text block. Supports markdown formatting.</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>intro</t>
+  </si>
+  <si>
+    <t>Year of entry.</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>Link to publication</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>The first version of the Pan-European Indoor Radon Map</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>mother tongue</t>
+  </si>
+  <si>
+    <t>fluent. It has been my everyday work language since 2016</t>
+  </si>
+  <si>
+    <t>R-Shiny</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>orcid</t>
+  </si>
+  <si>
+    <t>[ORCID](https://orcid.org/0000-0003-0624-2345)</t>
+  </si>
+  <si>
+    <t>Name of package</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Description of the package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description   </t>
+  </si>
+  <si>
+    <t>dangeo</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/dangeo.git</t>
+  </si>
+  <si>
+    <t>ggpyramid</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/ggpyramid.git</t>
+  </si>
+  <si>
+    <t>ggrugby</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/ggrugby.git</t>
+  </si>
+  <si>
+    <t>safecastR</t>
+  </si>
+  <si>
+    <t>https://github.com/javiereliomedina/safecastR.git</t>
+  </si>
+  <si>
+    <t>R package for accessing the Danish Map Supply Download via the kortforsyningen FTP</t>
+  </si>
+  <si>
+    <t>R function for plotting population pyramids in {ggplot2}</t>
+  </si>
+  <si>
+    <t>R functions for plotting rugby events in {ggplot2}</t>
+  </si>
+  <si>
+    <t>R package for loading data from Safecast API</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>Name of App</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>Description of the app</t>
+  </si>
+  <si>
+    <t>CV_app</t>
+  </si>
+  <si>
+    <t>Shiny app for building data-driven CVs from Excel files</t>
+  </si>
+  <si>
+    <t>https://javierelio.shinyapps.io/cv_app/</t>
+  </si>
+  <si>
+    <t>DK_migr</t>
+  </si>
+  <si>
+    <t>Shiny app for analysisng  migration data from Statistic Denmark</t>
+  </si>
+  <si>
+    <t>https://javierelio.shinyapps.io/DK_migr_app/</t>
+  </si>
+  <si>
+    <t>Geoinformatics: Spatial Data Science 1</t>
+  </si>
+  <si>
+    <t>A hands-on data science session in Python to train skills in data science-related tasks. Aalborg University</t>
+  </si>
+  <si>
+    <t>Practical exercise: a new indoor radon risk map of Ireland. Geology, School of Natural Sciences, Trinity College Dublin, School of Natural Sciences, Geology</t>
+  </si>
+  <si>
+    <t>Migration studies with a Compositional Data approach: a case study of population structure in the Capital Region of Denmark</t>
+  </si>
+  <si>
+    <t>ArXiv</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2201.02451v1</t>
+  </si>
+  <si>
+    <t>Behaviour of smoldering fires during periodic refilling of wood pellets into silos</t>
+  </si>
+  <si>
+    <t>Journal of Loss Prevention in the Process Industries</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.jlp.2021.104565</t>
+  </si>
+  <si>
+    <t>Hubs and clusters approach to unlock the development of carbon capture and storage – Case study in Spain</t>
+  </si>
+  <si>
+    <t>Applied Energy</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.apenergy.2021.117418</t>
+  </si>
+  <si>
+    <t>Development of a geogenic radon hazard index—concept, history, experiences</t>
+  </si>
+  <si>
+    <t>International Journal of Environmental Research and Public Health,</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.3390/ijerph17114134</t>
+  </si>
+  <si>
+    <t>Preliminary Results From Detection of Microplastics in Liquid Samples Using Flow Cytometry</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.3389/fmars.2020.552688</t>
+  </si>
+  <si>
+    <t>The Campo de Calatrava Volcanic Field (central Spain): Fluid geochemistry in a CO2‑rich area</t>
+  </si>
+  <si>
+    <t>Applied Geochemistry</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.apgeochem.2019.01.011</t>
+  </si>
+  <si>
+    <t>Rapid radon potential classification using soil‑gas radon measurements in the Cooley Peninsula, County Louth, Ireland</t>
+  </si>
+  <si>
+    <t>Environmental Earth Sciences</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1007/s12665-019-8339-4</t>
+  </si>
+  <si>
+    <t>Applicability of radon emanometry in lithologically discontinuous sites contaminated by organic chemicals</t>
+  </si>
+  <si>
+    <t>Environmental Science and Pollution Research</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1007/s11356-018-2372-9</t>
+  </si>
+  <si>
+    <t>Environmental risk assessment of cobalt and manganese from industrial sources in an estuarine system</t>
+  </si>
+  <si>
+    <t>Environmental Geochemistry and Health</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1007/s10653-017-0020-9</t>
+  </si>
+  <si>
+    <t>A multi‑statistical approach for estimating the total output of CO2 from diffuse soil degassing by the accumulation chamber method</t>
+  </si>
+  <si>
+    <t>International Journal of Greenhouse Gas Control</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2016.02.012</t>
+  </si>
+  <si>
+    <t>Evaluation of the applicability of four different radon measurement techniques for monitoring CO2 storage sites</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2015.06.021</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2014.10.014</t>
+  </si>
+  <si>
+    <t>Systematic approach for the selection of monitoring technologies in CO2 geological storage projects, aplication of multicriteria decision making</t>
+  </si>
+  <si>
+    <t>Global Nest Journal</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.30955/gnj.001241</t>
+  </si>
+  <si>
+    <t>Gas monitoring methodology and application to CCS projects as defined by atmospheric and remote sensing survey in the natural analogue of campo de Calatrava</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.30955/gnj.001242</t>
+  </si>
+  <si>
+    <t>Origin of the gases released from the Acqua Passante and Ermeta wells (Mt. Amiata, central Italy) and possible environmental implications for their closure</t>
+  </si>
+  <si>
+    <t>Annals of Geophysics</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.4401/ag-6584</t>
+  </si>
+  <si>
+    <t>Gas Discharges for Continental Spain: Geochemical and Isotopic Features</t>
+  </si>
+  <si>
+    <t>Mineralogical Magazine</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1180/minmag.2013.077.5.22</t>
+  </si>
+  <si>
+    <t>Hydrogeochemistry of surface and spring waters in the surroundings of the CO2 injection site at Hontomín‑Huermeces (Burgos, Spain)</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2013.01.012</t>
+  </si>
+  <si>
+    <t>CO2 soil flux baseline at the technological development plant for CO2 injection at Hontomin (Burgos, Spain)</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2013.07.013</t>
+  </si>
+  <si>
+    <t>Sampling strategies using the ”accumulation chamber” for monitoring geological storage of CO2</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.ijggc.2012.04.006</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>List of authors</t>
+  </si>
+  <si>
+    <t>Elío, J., Georgati, M., Hansen, H.S., Keßler, C.</t>
+  </si>
+  <si>
+    <t>Fernandez‑Anez, N., Meyer, A.K., Elío, J., Kleppe, G., Hagen, B.C., Frette, V.</t>
+  </si>
+  <si>
+    <t>Sun, X., Alcalde, J., Bakhtbidar, M., Elío, J., Vilarrasa, V., Canal, J., Ballesteros, J., Heinemann, N., Haszeldine, S., Cavanagh, A., Vega‑Maza, D., Rubiera, F., Martínez‑Orio, R., Johnson, G., Carbonell, R., Marzan, I., Travé, A., Gomez‑Rivas, E.</t>
+  </si>
+  <si>
+    <t>Bossew, P., Cinelli, G., Ciotoli, G., Crowley, Q.G., de Cort, M., Elío, J., Gruber, V., Petermann, E.</t>
+  </si>
+  <si>
+    <t>Elío, J., Crowley, Q., Scanlon, R., Hodgson, J., Long, S., Cooper, M., Gallagher, V.</t>
+  </si>
+  <si>
+    <t>Kaile, N., Lindivat, M., Elío, J., Thuestad, G., Crowley, Q.G., Hoell, I.A.</t>
+  </si>
+  <si>
+    <t>Nisi, B., Vaselli, O., Elío, J., Giannini, L., Tassi, F., Guidi, M., Darrah, T.H., Maletic, E.L., Delgado Huertas, A., Marchionni, S.</t>
+  </si>
+  <si>
+    <t>Elío, J., Crowley, Q., Scanlon, R., Hodgson, J., Long, S.</t>
+  </si>
+  <si>
+    <t>Elío, J., Cinelli, G., Bossew, P., Gutiérrez‑Villanueva, J.L., Tollefsen, T., De Cort, M., Nogarotto, A., Braga, R.</t>
+  </si>
+  <si>
+    <t>De Miguel, E., Barrio‑Parra, F., Elío, J., Izquierdo‑Díaz, M., García‑González, J.E., Mazadiego, L.F., Medina, R.</t>
+  </si>
+  <si>
+    <t>Barrio‑Parra, F., Elío, J., De Miguel, E., García‑González, J.E., Izquierdo, M., Álvarez, R.</t>
+  </si>
+  <si>
+    <t>Elío, J., Crowley, Q., Scanlon, R., Hodgson, J., Zgaga, L.</t>
+  </si>
+  <si>
+    <t>Elío, J., Ortega, M.F., Nisi, B., Mazadiego, L.F., Vaselli, O., Caballero, J., Chacón, E.</t>
+  </si>
+  <si>
+    <t>Elío, J., Ortega, M.F., Nisi, B., Mazadiego, L.F., Vaselli, O., Caballero, J., Quindós‑Poncela, L.S., Sainz‑Fernández, C., Pous, J.</t>
+  </si>
+  <si>
+    <t>Elío, J., Ortega, M.F., Nisi, B., Mazadiego, L.F., Vaselli, O., Caballero, J., Grandia, F.</t>
+  </si>
+  <si>
+    <t>Llamas, B., Mazadiego, L.F., Elío, J., Ortega, M.F., Grandia, F., Rincones, M.</t>
+  </si>
+  <si>
+    <t>Ortega, M.F., Rincones, M., Elío, J., Del Olmo, G.J., Nisi, B., Mazadiego, L.F., Iglesias, L., Vaselli, O., Grandia, F., García, R., De La Vega, R., Llamas, B.</t>
+  </si>
+  <si>
+    <t>Nisi, B., Vaselli, O., Tassi, F., Elío, J., Ortega, M., Caballero, J., Rappuoli, D., Mazadiego, L.F.</t>
+  </si>
+  <si>
+    <t>Vaselli, O., Nisi, B., Tassi, F., Darrah, T., Bruno, J., Elío, J., Grandia, F., Del Villar, L.P.</t>
+  </si>
+  <si>
+    <t>Nisi, B., Vaselli, O., Tassi, F., Elío, J., Huertas, A.D., Mazadiego, L.F., Ortega, M.F.</t>
+  </si>
+  <si>
+    <t>Elío, J., Nisi, B., Ortega, M.F., Mazadiego, L.F., Vaselli, O., Grandia, F.</t>
+  </si>
+  <si>
+    <t>Elío, J., Ortega, M.F., Chacón, E., Mazadiego, L.F., Grandia, F.</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>Cinelli, G., De Cort, M., Tollefsen, T. (Eds.)</t>
+  </si>
+  <si>
+    <t>European Atlas of Natural Radiation</t>
+  </si>
+  <si>
+    <t>Publication Office of the European Union</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.2760/520053</t>
+  </si>
+  <si>
+    <t>Elío, J., Ortega, M.F., Mazadiego, L.F., Nisi, B., Vaselli, O., Garcia‑Martinez, M.J.</t>
+  </si>
+  <si>
+    <t>Monitoring of soil gases in the characterization stage of CO2 storage in saline aquifers and possible effects of CO2 leakages in the groundwater system</t>
+  </si>
+  <si>
+    <t>Geologic Carbon Sequestration: Understanding Reservoir Behavior</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1007/978-3-319-27019-7_5</t>
+  </si>
+  <si>
+    <t>An All‑Ireland Geogenic Indoor Radon Map</t>
+  </si>
+  <si>
+    <t>Radon monitoring and hazard prediction in Ireland</t>
+  </si>
+  <si>
+    <t>Geological Survey Ireland</t>
+  </si>
+  <si>
+    <t>Irish Research Council ‑ Enterprise Partnership Scheme Fellowship 2015</t>
+  </si>
+  <si>
+    <t>Primary institution affiliation for entry (or funding body for projects)</t>
+  </si>
+  <si>
+    <t>Roland Schlich Early Career Scientist’s Travel Support grant</t>
+  </si>
+  <si>
+    <t>European Geosciences Union</t>
+  </si>
+  <si>
+    <t>European Radon Association Award</t>
+  </si>
+  <si>
+    <t>European Radon Association</t>
+  </si>
+  <si>
+    <t>Extraordinary PhD Award</t>
+  </si>
+  <si>
+    <t>Gómez‑Pardo Foundation Award</t>
+  </si>
+  <si>
+    <t>Spanish Royal Academy of Doctors</t>
+  </si>
+  <si>
+    <t>International Mobility Program Grant</t>
+  </si>
+  <si>
+    <t>Social Council at the Technical University of Madrid</t>
+  </si>
+  <si>
+    <t>Doctoral Research Grant</t>
+  </si>
+  <si>
+    <t>Ciudad de la Energía Foundation</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>International Atomic Energy Agency</t>
+  </si>
+  <si>
+    <t>European Commission ‑ Joint Research Centre</t>
+  </si>
+  <si>
+    <t>membership</t>
+  </si>
+  <si>
+    <t>Visiting Research Assistant</t>
+  </si>
+  <si>
+    <t>Research Stay</t>
+  </si>
+  <si>
+    <t>University of Florence, Dipartimento di Scienze della Terra</t>
+  </si>
+  <si>
+    <t>Florence, IT</t>
+  </si>
+  <si>
+    <t>Geological residential field-school</t>
+  </si>
+  <si>
+    <t>GIS module in MSc Environmental Science</t>
+  </si>
+  <si>
+    <t>Massive Online Course ‑ MOOC</t>
+  </si>
+  <si>
+    <t>Monitoring CO2 geological storage sites, Technical University of
+Madrid</t>
+  </si>
+  <si>
+    <t>Michaelmas Semester 2016 ‑ Geology Seminar Series</t>
+  </si>
+  <si>
+    <t>Modelling Indoor Radon Concentration: Towards a High‑Resolution Indoor Radon Map of Ireland, Trinity College Dublin, School of Natural Sciences, Geology</t>
+  </si>
+  <si>
+    <t>Summer school in Carbon Capture and Storage</t>
+  </si>
+  <si>
+    <t>Surface and subsurface monitoring of a CO2 storage site: theory and practice, University of León</t>
+  </si>
+  <si>
+    <t>I have worked in a variety of roles ranging from journalist to software engineer to data scientist. I like collaborative environments where I can learn from my peers.</t>
+  </si>
+  <si>
+    <t>I am passionate about education. I believe that no topic is too complex if the teacher is empathetic and willing to think about new methods of approaching task.</t>
+  </si>
+  <si>
+    <t>I regularly blog about data science and visualization on my blog [LiveFreeOrDichotomize.](https://livefreeordichotomize.com/)</t>
+  </si>
+  <si>
+    <t>publications_aside</t>
+  </si>
+  <si>
+    <t>teaching_aside</t>
+  </si>
+  <si>
+    <t>experience_aside</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>award</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>inv_position</t>
+  </si>
+  <si>
+    <t>Applied Marine Microbiology</t>
+  </si>
+  <si>
+    <t>Western Norway University of Applied Sciences</t>
+  </si>
+  <si>
+    <t>European Geogenic Radon Map expert group</t>
+  </si>
+  <si>
+    <t>Ispra, IT</t>
+  </si>
+  <si>
+    <t>Brussels, BE</t>
+  </si>
+  <si>
+    <t>supervision</t>
+  </si>
+  <si>
+    <t>Co‑supervisor of a Master thesis in Environmental Sciences</t>
+  </si>
+  <si>
+    <t>Co‑supervisor of an Earth Science Dissertation</t>
+  </si>
+  <si>
+    <t>Trinity College Dublin, School of Natural Sciences, Geology</t>
+  </si>
+  <si>
+    <t>Assessing the contribution of Quaternary deposits to the soil radon budget in Ireland</t>
+  </si>
+  <si>
+    <t>Evaluating two techniques of soil gas radon detection in application, performance and against indoor radon concentrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinity College Dublin, School of Natural Sciences, Geology </t>
+  </si>
+  <si>
+    <t>Linking radon concentrations between the natural and built environments</t>
+  </si>
+  <si>
+    <t>ext_sensor</t>
+  </si>
+  <si>
+    <t>External PhD examiner</t>
+  </si>
+  <si>
+    <t>Thesis: “Integration of remote sensing and statistical techniques for detecting CO2 leaks in geological storage areas through the study of natural analogues</t>
+  </si>
+  <si>
+    <t>short_description</t>
+  </si>
+  <si>
+    <t>Expert on environmental research, statistics, spatial data analysis, and modelling</t>
+  </si>
+  <si>
+    <t>Natural hazards and climate change; Environmental risk assessment; Statistics, spatial data analysis, and geostatistics; Geographic information systems; R language</t>
+  </si>
+  <si>
+    <t>research_interests</t>
+  </si>
+  <si>
+    <t>I am an engineer with 15+ years of research and teaching experience, with a solid background in statistics, spatial data analysis, and modelling. My main research area is environmental science, with a particular interest in natural hazards and climate change.</t>
+  </si>
+  <si>
+    <t>Vienna, AT</t>
+  </si>
+  <si>
+    <t>Regional Workshop on Development of Radon Maps and the Definition of Radon‑Prone Areas</t>
+  </si>
+  <si>
     <t>Vilnius, LT</t>
   </si>
   <si>
+    <t>Expert Mission on radon regulations implementation</t>
+  </si>
+  <si>
+    <t>Nicosia, CY</t>
+  </si>
+  <si>
     <t>Expert Mission to advice on radon detection, mapping and analysis</t>
   </si>
   <si>
     <t>Lima, PE</t>
   </si>
   <si>
-    <t>Geological residential field-school.</t>
-  </si>
-  <si>
-    <t>Teaching assistant, 10 day geological residential fieldschool in SE Spain, Trinity College Dublin, School of Natural Sciences, Geology</t>
-  </si>
-  <si>
-    <t>GIS module in MSc Environmental Science.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application of airborne radiometric surveys for large scale geogenic radon potential classification </t>
-  </si>
-  <si>
-    <t>Journal of the European Radon Association</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.35815/radon.v1.4358</t>
-  </si>
-  <si>
-    <t>Natural Hazards and Earth System Sciences</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.5194/nhess-19-2451-2019</t>
-  </si>
-  <si>
-    <t>Estimation of residential radon exposure and definition of Radon Priority Areas based on expected lung cancer incidence</t>
-  </si>
-  <si>
-    <t>Environment International</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1016/j.envint.2018.02.025</t>
-  </si>
-  <si>
-    <t>Logistic regression model for detecting radon prone areas in Ireland</t>
-  </si>
-  <si>
-    <t>Science of the Total Environment</t>
-  </si>
-  <si>
-    <t>http://dx.doi.org/10.1016/j.scitotenv.2017.05.071</t>
-  </si>
-  <si>
-    <t>Name of language</t>
-  </si>
-  <si>
-    <t>Relative numeric level of skill</t>
-  </si>
-  <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>ArcGIS</t>
-  </si>
-  <si>
-    <t>QGIS</t>
-  </si>
-  <si>
-    <t>Id used for finding text block</t>
-  </si>
-  <si>
-    <t>Contents of text block. Supports markdown formatting.</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>intro</t>
-  </si>
-  <si>
-    <t>Year of entry.</t>
-  </si>
-  <si>
-    <t>doi</t>
-  </si>
-  <si>
-    <t>Link to publication</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>journal</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>article</t>
-  </si>
-  <si>
-    <t>The first version of the Pan-European Indoor Radon Map</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>mother tongue</t>
-  </si>
-  <si>
-    <t>fluent. It has been my everyday work language since 2016</t>
-  </si>
-  <si>
-    <t>R-Shiny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional Workshop on Development of Radon Maps and the Definition of Radon Prone Areas </t>
-  </si>
-  <si>
-    <t>I am an engineer with 10+ years of research and teaching experience, with a solid background in statistics, spatial data analysis, and modelling. My main research area is environmental science, with a particular interest in natural hazards and climate change.</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>orcid</t>
-  </si>
-  <si>
-    <t>[ORCID](https://orcid.org/0000-0003-0624-2345)</t>
-  </si>
-  <si>
-    <t>Name of package</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Description of the package</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description   </t>
-  </si>
-  <si>
-    <t>dangeo</t>
-  </si>
-  <si>
-    <t>https://github.com/javiereliomedina/dangeo.git</t>
-  </si>
-  <si>
-    <t>ggpyramid</t>
-  </si>
-  <si>
-    <t>https://github.com/javiereliomedina/ggpyramid.git</t>
-  </si>
-  <si>
-    <t>ggrugby</t>
-  </si>
-  <si>
-    <t>https://github.com/javiereliomedina/ggrugby.git</t>
-  </si>
-  <si>
-    <t>safecastR</t>
-  </si>
-  <si>
-    <t>https://github.com/javiereliomedina/safecastR.git</t>
-  </si>
-  <si>
-    <t>R package for accessing the Danish Map Supply Download via the kortforsyningen FTP</t>
-  </si>
-  <si>
-    <t>R function for plotting population pyramids in {ggplot2}</t>
-  </si>
-  <si>
-    <t>R functions for plotting rugby events in {ggplot2}</t>
-  </si>
-  <si>
-    <t>R package for loading data from Safecast API</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
-    <t>Name of App</t>
-  </si>
-  <si>
-    <t>app</t>
-  </si>
-  <si>
-    <t>Description of the app</t>
-  </si>
-  <si>
-    <t>CV_app</t>
-  </si>
-  <si>
-    <t>Shiny app for building data-driven CVs from Excel files</t>
-  </si>
-  <si>
-    <t>https://javierelio.shinyapps.io/cv_app/</t>
-  </si>
-  <si>
-    <t>DK_migr</t>
-  </si>
-  <si>
-    <t>Shiny app for analysisng  migration data from Statistic Denmark</t>
-  </si>
-  <si>
-    <t>https://javierelio.shinyapps.io/DK_migr_app/</t>
-  </si>
-  <si>
-    <t>Geoinformatics: Spatial Data Science 1</t>
-  </si>
-  <si>
-    <t>A hands-on data science session in Python to train skills in data science-related tasks. Aalborg University</t>
-  </si>
-  <si>
-    <t>Practical exercise: a new indoor radon risk map of Ireland. Geology, School of Natural Sciences, Trinity College Dublin, School of Natural Sciences, Geology</t>
-  </si>
-  <si>
-    <t>Expert, International Atomic Energy Agency</t>
+    <t>Working Group Meeting on Indoor Radon Dose</t>
+  </si>
+  <si>
+    <t>CO2 and Rn degassing from the natural analog of Campo de Calatrava (Spain): Implications for monitoring of CO2 storage sites</t>
   </si>
 </sst>
 </file>
@@ -779,7 +1215,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,13 +1299,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -891,23 +1327,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -915,41 +1351,78 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="121.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="135.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -960,71 +1433,74 @@
         <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>2022</v>
       </c>
       <c r="F3">
-        <v>2013</v>
+        <v>2022</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1032,19 +1508,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>236</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="E4">
+        <v>2018</v>
       </c>
       <c r="F4">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -1052,19 +1531,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>237</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <v>2017</v>
       </c>
       <c r="F5">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -1072,19 +1554,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>2017</v>
       </c>
       <c r="F6">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -1092,19 +1577,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>2016</v>
       </c>
       <c r="F7">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1112,139 +1600,172 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>240</v>
       </c>
       <c r="C8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
+      <c r="E8">
+        <v>2016</v>
       </c>
       <c r="F8">
         <v>2016</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>2013</v>
       </c>
       <c r="F9">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>259</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>262</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="E10">
+        <v>2017</v>
       </c>
       <c r="F10">
-        <v>2009</v>
+        <v>2017</v>
+      </c>
+      <c r="G10" t="s">
+        <v>263</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>259</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>262</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="E11">
+        <v>2017</v>
       </c>
       <c r="F11">
-        <v>2007</v>
+        <v>2017</v>
+      </c>
+      <c r="G11" t="s">
+        <v>264</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>2016</v>
       </c>
       <c r="F12">
-        <v>2005</v>
+        <v>2016</v>
+      </c>
+      <c r="G12" t="s">
+        <v>266</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>267</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>268</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>2017</v>
       </c>
       <c r="F13">
-        <v>2019</v>
+        <v>2017</v>
+      </c>
+      <c r="G13" t="s">
+        <v>269</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="E14">
+        <v>2020</v>
       </c>
       <c r="F14">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -1252,19 +1773,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>48</v>
+      </c>
+      <c r="E15">
+        <v>2019</v>
       </c>
       <c r="F15">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
@@ -1272,19 +1796,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="E16">
+        <v>2016</v>
       </c>
       <c r="F16">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
@@ -1292,19 +1819,22 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <v>2014</v>
       </c>
       <c r="F17">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
@@ -1312,25 +1842,520 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>2009</v>
       </c>
       <c r="F18">
-        <v>2022</v>
+        <v>2013</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>2007</v>
+      </c>
+      <c r="F19">
+        <v>2009</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>2005</v>
+      </c>
+      <c r="F20">
+        <v>2007</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>2009</v>
+      </c>
+      <c r="F21">
+        <v>2013</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>2007</v>
+      </c>
+      <c r="F22">
+        <v>2009</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>1998</v>
+      </c>
+      <c r="F23">
+        <v>2005</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24">
+        <v>2017</v>
+      </c>
+      <c r="F24">
+        <v>2018</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25">
+        <v>2016</v>
+      </c>
+      <c r="F25">
+        <v>2017</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" t="s">
+        <v>218</v>
+      </c>
+      <c r="D26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26">
+        <v>2019</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>251</v>
+      </c>
+      <c r="B27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" t="s">
+        <v>258</v>
+      </c>
+      <c r="E27">
+        <v>2019</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28">
+        <v>2016</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>251</v>
+      </c>
+      <c r="B29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" t="s">
+        <v>223</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29">
+        <v>2014</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>251</v>
+      </c>
+      <c r="B30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>2012</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31">
+        <v>2009</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" t="s">
+        <v>228</v>
+      </c>
+      <c r="C32" t="s">
+        <v>229</v>
+      </c>
+      <c r="D32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E32">
+        <v>2019</v>
+      </c>
+      <c r="F32">
+        <v>2019</v>
+      </c>
+      <c r="G32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>252</v>
+      </c>
+      <c r="B33" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" t="s">
+        <v>229</v>
+      </c>
+      <c r="D33" t="s">
+        <v>279</v>
+      </c>
+      <c r="E33">
+        <v>2018</v>
+      </c>
+      <c r="F33">
+        <v>2018</v>
+      </c>
+      <c r="G33" t="s">
+        <v>278</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>252</v>
+      </c>
+      <c r="B34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" t="s">
+        <v>281</v>
+      </c>
+      <c r="E34">
+        <v>2018</v>
+      </c>
+      <c r="F34">
+        <v>2018</v>
+      </c>
+      <c r="G34" t="s">
+        <v>280</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" t="s">
+        <v>230</v>
+      </c>
+      <c r="D35" t="s">
+        <v>257</v>
+      </c>
+      <c r="E35">
+        <v>2018</v>
+      </c>
+      <c r="F35">
+        <v>2018</v>
+      </c>
+      <c r="G35" t="s">
+        <v>282</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" t="s">
+        <v>254</v>
+      </c>
+      <c r="C36" t="s">
+        <v>255</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36">
+        <v>2019</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" t="s">
+        <v>256</v>
+      </c>
+      <c r="C37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D37" t="s">
+        <v>257</v>
+      </c>
+      <c r="E37">
+        <v>2017</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" t="s">
+        <v>220</v>
+      </c>
+      <c r="D38" t="s">
+        <v>258</v>
+      </c>
+      <c r="E38">
+        <v>2016</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>253</v>
+      </c>
+      <c r="B39" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39">
+        <v>2018</v>
+      </c>
+      <c r="F39">
+        <v>2018</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" t="s">
+        <v>233</v>
+      </c>
+      <c r="C40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E40">
+        <v>2013</v>
+      </c>
+      <c r="F40">
+        <v>2013</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J23">
+    <sortCondition descending="1" ref="A3:A23"/>
+    <sortCondition descending="1" ref="F3:F23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -1348,23 +2373,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1372,7 +2397,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -1380,7 +2405,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1388,7 +2413,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>3.5</v>
@@ -1396,7 +2421,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B7">
         <v>2.5</v>
@@ -1408,151 +2433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3">
-        <v>2020</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4">
-        <v>2019</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5">
-        <v>2018</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6">
-        <v>2017</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:XFD6"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,39 +2448,684 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" customWidth="1"/>
+    <col min="3" max="3" width="140.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3">
+        <v>2012</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4">
+        <v>2013</v>
+      </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5">
+        <v>2013</v>
+      </c>
+      <c r="F5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6">
+        <v>2013</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7">
+        <v>2014</v>
+      </c>
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8">
+        <v>2014</v>
+      </c>
+      <c r="F8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9">
+        <v>2014</v>
+      </c>
+      <c r="F9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10">
+        <v>2015</v>
+      </c>
+      <c r="F10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11">
+        <v>2016</v>
+      </c>
+      <c r="F11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12">
+        <v>2016</v>
+      </c>
+      <c r="F12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13">
+        <v>2017</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14">
+        <v>2018</v>
+      </c>
+      <c r="F14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16">
+        <v>2018</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17">
+        <v>2019</v>
+      </c>
+      <c r="F17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18">
+        <v>2019</v>
+      </c>
+      <c r="F18" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19">
+        <v>2019</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" t="s">
+        <v>204</v>
+      </c>
+      <c r="C20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20">
+        <v>2019</v>
+      </c>
+      <c r="F20" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <v>2020</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22">
+        <v>2020</v>
+      </c>
+      <c r="F22" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23">
+        <v>2020</v>
+      </c>
+      <c r="F23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24">
+        <v>2021</v>
+      </c>
+      <c r="F24" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25">
+        <v>2021</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26">
+        <v>2022</v>
+      </c>
+      <c r="F26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>195</v>
+      </c>
+      <c r="C27" t="s">
+        <v>283</v>
+      </c>
+      <c r="D27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27">
+        <v>2015</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G26">
+    <sortCondition ref="E3:E26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1604,7 +3134,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1615,21 +3145,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1637,46 +3167,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1699,21 +3229,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1721,24 +3251,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Render full cv from excel (awersomeCV)
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="669" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C0B95F8-DE01-49C4-8E44-45819BE16291}"/>
+  <xr:revisionPtr revIDLastSave="687" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6A08C4F-33E5-4925-A107-50CA1B087676}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="1164" windowWidth="13596" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact_info" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="291">
   <si>
     <t>Id of contact section</t>
   </si>
@@ -880,13 +880,34 @@
   </si>
   <si>
     <t>CO2 and Rn degassing from the natural analog of Campo de Calatrava (Spain): Implications for monitoring of CO2 storage sites</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>User value for long CV</t>
+  </si>
+  <si>
+    <t>javiereliomedina</t>
+  </si>
+  <si>
+    <t>javierelio.netlify.app</t>
+  </si>
+  <si>
+    <t>+45 9940 2528</t>
+  </si>
+  <si>
+    <t>0000-0003-0624-2345</t>
+  </si>
+  <si>
+    <t>elio_javi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,6 +919,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1212,15 +1239,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1228,10 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1239,21 +1269,27 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1261,10 +1297,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1272,10 +1311,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1283,10 +1325,13 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1294,21 +1339,27 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1316,12 +1367,20 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{4C7E15E0-CC84-4A12-93B3-24E8D7A89D83}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{3154C355-2078-46F7-9885-FE2E4B4359E0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2488,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1) Update introduction. 2) Add space after short description in full CV.
</commit_message>
<xml_diff>
--- a/CV_data.xlsx
+++ b/CV_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="687" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6A08C4F-33E5-4925-A107-50CA1B087676}"/>
+  <xr:revisionPtr revIDLastSave="690" documentId="11_0D8161381A25DE2363B5874E3D6159398F9561EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85A4330F-4FA7-46EB-8DC7-6A74F8586BF2}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="1164" windowWidth="13596" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>Icon used from font-awesome 4 to label this contact section</t>
   </si>
   <si>
-    <t>The actual value written for the contact entry</t>
-  </si>
-  <si>
     <t>loc</t>
   </si>
   <si>
@@ -901,6 +898,9 @@
   </si>
   <si>
     <t>elio_javi</t>
+  </si>
+  <si>
+    <t>The actual value written for the contact entry (sort CV)</t>
   </si>
 </sst>
 </file>
@@ -1242,10 +1242,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1255,122 +1259,122 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>286</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>289</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1399,66 +1403,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
         <v>270</v>
-      </c>
-      <c r="B4" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -1486,74 +1490,74 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
         <v>127</v>
       </c>
-      <c r="C3" t="s">
-        <v>128</v>
-      </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>2022</v>
@@ -1567,16 +1571,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>2018</v>
@@ -1590,16 +1594,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <v>2017</v>
@@ -1613,16 +1617,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" t="s">
         <v>238</v>
       </c>
-      <c r="C6" t="s">
-        <v>239</v>
-      </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6">
         <v>2017</v>
@@ -1636,16 +1640,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>2016</v>
@@ -1659,16 +1663,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" t="s">
         <v>240</v>
       </c>
-      <c r="C8" t="s">
-        <v>241</v>
-      </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>2016</v>
@@ -1682,16 +1686,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" t="s">
         <v>242</v>
       </c>
-      <c r="C9" t="s">
-        <v>243</v>
-      </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9">
         <v>2013</v>
@@ -1705,16 +1709,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" t="s">
         <v>259</v>
       </c>
-      <c r="B10" t="s">
-        <v>260</v>
-      </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>2017</v>
@@ -1723,7 +1727,7 @@
         <v>2017</v>
       </c>
       <c r="G10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1731,16 +1735,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" t="s">
         <v>261</v>
       </c>
-      <c r="C11" t="s">
-        <v>262</v>
-      </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11">
         <v>2017</v>
@@ -1749,7 +1753,7 @@
         <v>2017</v>
       </c>
       <c r="G11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1757,16 +1761,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" t="s">
         <v>259</v>
       </c>
-      <c r="B12" t="s">
-        <v>260</v>
-      </c>
       <c r="C12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>2016</v>
@@ -1775,7 +1779,7 @@
         <v>2016</v>
       </c>
       <c r="G12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1783,16 +1787,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" t="s">
         <v>267</v>
       </c>
-      <c r="B13" t="s">
-        <v>268</v>
-      </c>
       <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
       </c>
       <c r="E13">
         <v>2017</v>
@@ -1801,7 +1805,7 @@
         <v>2017</v>
       </c>
       <c r="G13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -1809,16 +1813,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
       </c>
       <c r="E14">
         <v>2020</v>
@@ -1832,16 +1836,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
       </c>
       <c r="E15">
         <v>2019</v>
@@ -1855,16 +1859,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
       <c r="E16">
         <v>2016</v>
@@ -1878,16 +1882,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17">
         <v>2014</v>
@@ -1901,16 +1905,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
       </c>
       <c r="E18">
         <v>2009</v>
@@ -1924,16 +1928,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>2007</v>
@@ -1947,16 +1951,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <v>2005</v>
@@ -1970,16 +1974,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
       </c>
       <c r="E21">
         <v>2009</v>
@@ -1993,16 +1997,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
       </c>
       <c r="E22">
         <v>2007</v>
@@ -2016,16 +2020,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
       </c>
       <c r="E23">
         <v>1998</v>
@@ -2039,16 +2043,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24">
         <v>2017</v>
@@ -2062,16 +2066,16 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25">
         <v>2016</v>
@@ -2085,16 +2089,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" t="s">
         <v>217</v>
       </c>
-      <c r="C26" t="s">
-        <v>218</v>
-      </c>
       <c r="D26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E26">
         <v>2019</v>
@@ -2105,16 +2109,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C27" t="s">
         <v>219</v>
       </c>
-      <c r="C27" t="s">
-        <v>220</v>
-      </c>
       <c r="D27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E27">
         <v>2019</v>
@@ -2125,16 +2129,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
         <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>39</v>
       </c>
       <c r="E28">
         <v>2016</v>
@@ -2145,16 +2149,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" t="s">
         <v>222</v>
       </c>
-      <c r="C29" t="s">
-        <v>223</v>
-      </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E29">
         <v>2014</v>
@@ -2165,16 +2169,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B30" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" t="s">
         <v>224</v>
       </c>
-      <c r="C30" t="s">
-        <v>225</v>
-      </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>2012</v>
@@ -2185,16 +2189,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B31" t="s">
+        <v>225</v>
+      </c>
+      <c r="C31" t="s">
         <v>226</v>
       </c>
-      <c r="C31" t="s">
-        <v>227</v>
-      </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <v>2009</v>
@@ -2205,16 +2209,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32" t="s">
         <v>228</v>
       </c>
-      <c r="C32" t="s">
-        <v>229</v>
-      </c>
       <c r="D32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E32">
         <v>2019</v>
@@ -2223,7 +2227,7 @@
         <v>2019</v>
       </c>
       <c r="G32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
@@ -2231,16 +2235,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" t="s">
         <v>228</v>
       </c>
-      <c r="C33" t="s">
-        <v>229</v>
-      </c>
       <c r="D33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E33">
         <v>2018</v>
@@ -2249,7 +2253,7 @@
         <v>2018</v>
       </c>
       <c r="G33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -2257,16 +2261,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" t="s">
         <v>228</v>
       </c>
-      <c r="C34" t="s">
-        <v>229</v>
-      </c>
       <c r="D34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E34">
         <v>2018</v>
@@ -2275,7 +2279,7 @@
         <v>2018</v>
       </c>
       <c r="G34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -2283,16 +2287,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E35">
         <v>2018</v>
@@ -2301,7 +2305,7 @@
         <v>2018</v>
       </c>
       <c r="G35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
@@ -2309,16 +2313,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" t="s">
         <v>254</v>
       </c>
-      <c r="C36" t="s">
-        <v>255</v>
-      </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36">
         <v>2019</v>
@@ -2329,16 +2333,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s">
+        <v>255</v>
+      </c>
+      <c r="C37" t="s">
+        <v>229</v>
+      </c>
+      <c r="D37" t="s">
         <v>256</v>
-      </c>
-      <c r="C37" t="s">
-        <v>230</v>
-      </c>
-      <c r="D37" t="s">
-        <v>257</v>
       </c>
       <c r="E37">
         <v>2017</v>
@@ -2349,13 +2353,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E38">
         <v>2016</v>
@@ -2366,16 +2370,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
         <v>50</v>
-      </c>
-      <c r="D39" t="s">
-        <v>51</v>
       </c>
       <c r="E39">
         <v>2018</v>
@@ -2389,16 +2393,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B40" t="s">
+        <v>232</v>
+      </c>
+      <c r="C40" t="s">
         <v>233</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>234</v>
-      </c>
-      <c r="D40" t="s">
-        <v>235</v>
       </c>
       <c r="E40">
         <v>2013</v>
@@ -2432,23 +2436,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -2456,7 +2460,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -2464,7 +2468,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -2472,7 +2476,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6">
         <v>3.5</v>
@@ -2480,7 +2484,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7">
         <v>2.5</v>
@@ -2507,34 +2511,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2564,68 +2568,68 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3">
         <v>2012</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2633,22 +2637,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
         <v>170</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
       </c>
       <c r="E4">
         <v>2013</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -2656,22 +2660,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5">
         <v>2013</v>
       </c>
       <c r="F5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -2679,22 +2683,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6">
         <v>2013</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -2702,22 +2706,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" t="s">
         <v>162</v>
-      </c>
-      <c r="D7" t="s">
-        <v>163</v>
       </c>
       <c r="E7">
         <v>2014</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -2725,22 +2729,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8">
         <v>2014</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -2748,22 +2752,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
         <v>167</v>
-      </c>
-      <c r="D9" t="s">
-        <v>168</v>
       </c>
       <c r="E9">
         <v>2014</v>
       </c>
       <c r="F9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -2771,22 +2775,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10">
         <v>2015</v>
       </c>
       <c r="F10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -2794,22 +2798,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
         <v>156</v>
-      </c>
-      <c r="D11" t="s">
-        <v>157</v>
       </c>
       <c r="E11">
         <v>2016</v>
       </c>
       <c r="F11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -2817,22 +2821,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" t="s">
         <v>208</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>209</v>
-      </c>
-      <c r="D12" t="s">
-        <v>210</v>
       </c>
       <c r="E12">
         <v>2016</v>
       </c>
       <c r="F12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -2840,22 +2844,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
         <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
       </c>
       <c r="E13">
         <v>2017</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -2863,22 +2867,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" t="s">
         <v>150</v>
-      </c>
-      <c r="D14" t="s">
-        <v>151</v>
       </c>
       <c r="E14">
         <v>2018</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -2886,22 +2890,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" t="s">
         <v>153</v>
-      </c>
-      <c r="D15" t="s">
-        <v>154</v>
       </c>
       <c r="E15">
         <v>2018</v>
       </c>
       <c r="F15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -2909,22 +2913,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
         <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
       </c>
       <c r="E16">
         <v>2018</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -2932,22 +2936,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" t="s">
         <v>147</v>
-      </c>
-      <c r="D17" t="s">
-        <v>148</v>
       </c>
       <c r="E17">
         <v>2019</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -2955,22 +2959,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
         <v>144</v>
-      </c>
-      <c r="D18" t="s">
-        <v>145</v>
       </c>
       <c r="E18">
         <v>2019</v>
       </c>
       <c r="F18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -2978,22 +2982,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" t="s">
         <v>90</v>
       </c>
-      <c r="B19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C19" t="s">
-        <v>91</v>
-      </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19">
         <v>2019</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -3001,22 +3005,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" t="s">
         <v>203</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>204</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>205</v>
-      </c>
-      <c r="D20" t="s">
-        <v>206</v>
       </c>
       <c r="E20">
         <v>2019</v>
       </c>
       <c r="F20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -3024,22 +3028,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
         <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
       </c>
       <c r="E21">
         <v>2020</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -3047,22 +3051,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" t="s">
         <v>139</v>
-      </c>
-      <c r="D22" t="s">
-        <v>140</v>
       </c>
       <c r="E22">
         <v>2020</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -3070,19 +3074,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23">
         <v>2020</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -3090,22 +3094,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" t="s">
         <v>133</v>
-      </c>
-      <c r="D24" t="s">
-        <v>134</v>
       </c>
       <c r="E24">
         <v>2021</v>
       </c>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -3113,22 +3117,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" t="s">
         <v>136</v>
-      </c>
-      <c r="D25" t="s">
-        <v>137</v>
       </c>
       <c r="E25">
         <v>2021</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -3136,22 +3140,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
         <v>130</v>
-      </c>
-      <c r="D26" t="s">
-        <v>131</v>
       </c>
       <c r="E26">
         <v>2022</v>
       </c>
       <c r="F26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -3159,22 +3163,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E27">
         <v>2015</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -3204,68 +3208,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
         <v>105</v>
-      </c>
-      <c r="B3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
         <v>107</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
         <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3288,46 +3292,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>